<commit_message>
Added entries of the files checked in - Smitha
</commit_message>
<xml_diff>
--- a/Development/Artifacts/Changes From 13 April.xlsx
+++ b/Development/Artifacts/Changes From 13 April.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>Bugzilla Ticket No</t>
   </si>
@@ -77,6 +77,85 @@
 curam.molsa.financial.eft.ministryLetterAddressLine1
 curam.molsa.financial.eft.printAmountInWords
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EJBServer\components\MOLSA_ar\tab\FamilyOfPrisoner\FamilyOfPrisonerProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\MaidAssistance\MaidAssistanceProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\DivorcedLady\DivorcedLadyProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\Widow\WidowProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\FamilyOfMissing\FamilyOfMissingPDProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\ExceptionCase\ExceptionCaseProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\DesertedWife\DesertedWifeProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\FamilyInNeed\FamilyInNeedPDProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\IncapableOfWorking\IncapableOfWorkingPDProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\AnonymousParents\AnonymousParentsPDProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\SeniorCitizen\SeniorCitizenPDProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\FamilyOfMissing\FamilyOfMissingProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\Handicap\HandicapPDProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\Orphan\OrphanPDProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\FamilyOfPrisoner\FamilyOfPrisonerPDProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\MaidAssistance\MaidAssistancePDProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\DivorcedLady\DivorcedLadyPDProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\Widow\WidowPDProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\FamilyInNeed\FamilyInNeedProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\ExceptionCase\ExceptionCasePDProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\DesertedWife\DesertedWifePDProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\IncapableOfWorking\IncapableOfWorkingProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\AnonymousParents\AnonymousParentsProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\SeniorCitizen\SeniorCitizenProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\Handicap\HandicapProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\Orphan\OrphanProductDisplay_ar.properties  
+</t>
+  </si>
+  <si>
+    <t>Smitha</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EJBServer\components\MOLSA\data\initial\blob\MOLSASMSMessageText.properties
+EJBServer\components\MOLSA_ar\data\initial\blob\MOLSASMSMessageTextArabic.properties
+</t>
+  </si>
+  <si>
+    <t>Properties were changed in English and Arabic</t>
+  </si>
+  <si>
+    <t>Upload the changed properties through  admin</t>
+  </si>
+  <si>
+    <t>Added new files for the Arabic translations
+upload the new properties</t>
+  </si>
+  <si>
+    <t>New entries were added to 
+EJBServer\components\MOLSA\data\initial\rules\CREOLEPRODUCTDECISIONDISPCAT.dmx
+EJBServer\components\MOLSA\data\initial\rules\CREOLEPRODUCTPERIODDISPCAT.dmx
+EJBServer\components\MOLSA\data\initial\rules\CREOLERULECLASSLINK.dmx
+EJBServer\components\MOLSA\CREOLE_Rule_Sets\ExceptionCaseDisplayRuleSet.xml
+New file added is
+EJBServer\components\MOLSA\CREOLE_Rule_Sets\SocialAssistance\ExceptionCase\ExceptionCaseUnitInformation.xml</t>
+  </si>
+  <si>
+    <t>Use build and upload ruleset to upload the ruleset
+Execute the mentioned SQL queries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+INSERT INTO CREOLEPRODUCTPERIODDISPCAT (CREOLEPRODUCTPERIODDISPCATID, CREOLEPRODUCTPERIODID, CREOLEPRODUCTDECISIONDISPCATID, DECISIONDETAILSRCLID, VERSIONNO) VALUES (4550, 4512, 4550, 4605, 1);
+INSERT INTO CREOLEPRODUCTDECISIONDISPCAT (CREOLEPRODUCTDECISIONDISPCATID, PRODUCTID, NAMEID, DISPLAYORDER, DISPLAYPAGENAME, CATEGORYREF, VERSIONNO) VALUES (4550, 45012, 4563, 3, 'None', 'unitInformation', 1);
+INSERT INTO CREOLERULECLASSLINK (CREOLERULECLASSLINKID, CREOLERULESETID, RULECLASSNAME, VERSIONNO) VALUES (4605, 4549, 'ExceptionCaseUnitInformation', 1);
+</t>
+  </si>
+  <si>
+    <t>EJBServer\components\MOLSA\source\curam\molsa\core\sl\impl\MOLSAEvidenceControllerInterfaceImpl.java</t>
+  </si>
+  <si>
+    <t>Added conditions</t>
+  </si>
+  <si>
+    <t>Changed the Class file.</t>
   </si>
 </sst>
 </file>
@@ -141,7 +220,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -154,6 +233,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,11 +540,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,11 +610,94 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D4" s="1"/>
+    <row r="3" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>42122</v>
+      </c>
+      <c r="B3">
+        <v>372</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C5" s="1"/>
+    <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>42122</v>
+      </c>
+      <c r="B4">
+        <v>371</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="360" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>42117</v>
+      </c>
+      <c r="B5">
+        <v>375</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>42118</v>
+      </c>
+      <c r="B6">
+        <v>376</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -546,6 +711,34 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">UQKZYU5EZKJQ-17-950</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">
+      <Url>https://dionatec.sharepoint.com/GlobalServices/_layouts/15/DocIdRedir.aspx?ID=UQKZYU5EZKJQ-17-950</Url>
+      <Description>UQKZYU5EZKJQ-17-950</Description>
+    </_dlc_DocIdUrl>
+    <SharedWithUsers xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -593,34 +786,6 @@
     <Filter/>
   </Receiver>
 </spe:Receivers>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">UQKZYU5EZKJQ-17-950</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">
-      <Url>https://dionatec.sharepoint.com/GlobalServices/_layouts/15/DocIdRedir.aspx?ID=UQKZYU5EZKJQ-17-950</Url>
-      <Description>UQKZYU5EZKJQ-17-950</Description>
-    </_dlc_DocIdUrl>
-    <SharedWithUsers xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -808,22 +973,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE6F0B25-6AD0-4AF9-AE4F-0D8285608470}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A3CD956-F256-4860-8B56-AE881D5ADEC8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1926F8BC-3749-487B-86BA-515B8CAD861D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -836,6 +985,22 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A3CD956-F256-4860-8B56-AE881D5ADEC8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE6F0B25-6AD0-4AF9-AE4F-0D8285608470}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>